<commit_message>
Saving changes to excel files.
</commit_message>
<xml_diff>
--- a/Sales_Marketing/Market_Campaign_ROI.xlsx
+++ b/Sales_Marketing/Market_Campaign_ROI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\ISYS40251_Deriving-Value-Data-Analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\ISYS40251_Deriving-Value-Data-Analytics\Sales_Marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B55BA2B-6B3D-45B0-A631-8958E365E834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381E8B39-FF60-4214-B38F-F16289B1758B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,11 +225,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F289"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -581,7 +584,7 @@
       <c r="E2">
         <v>5976</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>337.01472556894248</v>
       </c>
     </row>
@@ -601,7 +604,7 @@
       <c r="E3">
         <v>5102</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>789.18071344570762</v>
       </c>
     </row>
@@ -621,7 +624,7 @@
       <c r="E4">
         <v>5441</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>601.37842308399195</v>
       </c>
     </row>
@@ -641,7 +644,7 @@
       <c r="E5">
         <v>6184</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>494.97089262613201</v>
       </c>
     </row>
@@ -661,7 +664,7 @@
       <c r="E6">
         <v>6729</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>368.7323525040868</v>
       </c>
     </row>
@@ -681,7 +684,7 @@
       <c r="E7">
         <v>6188</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>465.69166127989661</v>
       </c>
     </row>
@@ -701,7 +704,7 @@
       <c r="E8">
         <v>6407</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>662.71265803027939</v>
       </c>
     </row>
@@ -721,7 +724,7 @@
       <c r="E9">
         <v>5199</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>748.08617041738796</v>
       </c>
     </row>
@@ -741,7 +744,7 @@
       <c r="E10">
         <v>6817</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>250.02200381399439</v>
       </c>
     </row>
@@ -761,7 +764,7 @@
       <c r="E11">
         <v>5230</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>610.82217973231354</v>
       </c>
     </row>
@@ -781,7 +784,7 @@
       <c r="E12">
         <v>5970</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>455.61139028475708</v>
       </c>
     </row>
@@ -801,7 +804,7 @@
       <c r="E13">
         <v>6894</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>715.63678561067593</v>
       </c>
     </row>
@@ -821,7 +824,7 @@
       <c r="E14">
         <v>5801</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>702.80986036890192</v>
       </c>
     </row>
@@ -841,7 +844,7 @@
       <c r="E15">
         <v>6523</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>250.71286217997849</v>
       </c>
     </row>
@@ -861,7 +864,7 @@
       <c r="E16">
         <v>6746</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>333.36792173139639</v>
       </c>
     </row>
@@ -881,7 +884,7 @@
       <c r="E17">
         <v>5987</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>430.81676966761319</v>
       </c>
     </row>
@@ -901,7 +904,7 @@
       <c r="E18">
         <v>6852</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>314.11266783420899</v>
       </c>
     </row>
@@ -921,7 +924,7 @@
       <c r="E19">
         <v>6655</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>460.15026296018038</v>
       </c>
     </row>
@@ -941,7 +944,7 @@
       <c r="E20">
         <v>5250</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>984.3047619047619</v>
       </c>
     </row>
@@ -961,7 +964,7 @@
       <c r="E21">
         <v>5084</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>788.84736428009444</v>
       </c>
     </row>
@@ -981,7 +984,7 @@
       <c r="E22">
         <v>6827</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>607.80723597480596</v>
       </c>
     </row>
@@ -1001,7 +1004,7 @@
       <c r="E23">
         <v>6616</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>623.00483675937119</v>
       </c>
     </row>
@@ -1021,7 +1024,7 @@
       <c r="E24">
         <v>5586</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>751.89760114572141</v>
       </c>
     </row>
@@ -1041,7 +1044,7 @@
       <c r="E25">
         <v>6492</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>251.10905730129389</v>
       </c>
     </row>
@@ -1061,7 +1064,7 @@
       <c r="E26">
         <v>5433</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>797.7728695011964</v>
       </c>
     </row>
@@ -1081,7 +1084,7 @@
       <c r="E27">
         <v>6650</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>692.63157894736844</v>
       </c>
     </row>
@@ -1101,7 +1104,7 @@
       <c r="E28">
         <v>6981</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>409.42558372725972</v>
       </c>
     </row>
@@ -1121,7 +1124,7 @@
       <c r="E29">
         <v>5651</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>410.38754202795963</v>
       </c>
     </row>
@@ -1141,7 +1144,7 @@
       <c r="E30">
         <v>5829</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>711.97460971007035</v>
       </c>
     </row>
@@ -1161,7 +1164,7 @@
       <c r="E31">
         <v>5320</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>451.78571428571428</v>
       </c>
     </row>
@@ -1181,7 +1184,7 @@
       <c r="E32">
         <v>6566</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>676.04325312214439</v>
       </c>
     </row>
@@ -1201,7 +1204,7 @@
       <c r="E33">
         <v>5808</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>736.1914600550964</v>
       </c>
     </row>
@@ -1221,7 +1224,7 @@
       <c r="E34">
         <v>6958</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>651.92584075883872</v>
       </c>
     </row>
@@ -1241,7 +1244,7 @@
       <c r="E35">
         <v>5108</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>601.44870790916207</v>
       </c>
     </row>
@@ -1261,7 +1264,7 @@
       <c r="E36">
         <v>6518</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>636.1153728137466</v>
       </c>
     </row>
@@ -1281,7 +1284,7 @@
       <c r="E37">
         <v>6923</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>607.98786653185039</v>
       </c>
     </row>
@@ -1301,7 +1304,7 @@
       <c r="E38">
         <v>6879</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>300.88675679604597</v>
       </c>
     </row>
@@ -1321,7 +1324,7 @@
       <c r="E39">
         <v>5430</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>814.64088397790044</v>
       </c>
     </row>
@@ -1341,7 +1344,7 @@
       <c r="E40">
         <v>6297</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>805.78053041130693</v>
       </c>
     </row>
@@ -1361,7 +1364,7 @@
       <c r="E41">
         <v>5472</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>823.19078947368428</v>
       </c>
     </row>
@@ -1381,7 +1384,7 @@
       <c r="E42">
         <v>6713</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>332.25085654699842</v>
       </c>
     </row>
@@ -1401,7 +1404,7 @@
       <c r="E43">
         <v>5701</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>466.79529907033861</v>
       </c>
     </row>
@@ -1421,7 +1424,7 @@
       <c r="E44">
         <v>5656</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2">
         <v>387.07567185289957</v>
       </c>
     </row>
@@ -1441,7 +1444,7 @@
       <c r="E45">
         <v>5203</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>588.81414568518164</v>
       </c>
     </row>
@@ -1461,7 +1464,7 @@
       <c r="E46">
         <v>5628</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="2">
         <v>740.9203980099503</v>
       </c>
     </row>
@@ -1481,7 +1484,7 @@
       <c r="E47">
         <v>6774</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>548.13994685562443</v>
       </c>
     </row>
@@ -1501,7 +1504,7 @@
       <c r="E48">
         <v>5622</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>685.18320882248304</v>
       </c>
     </row>
@@ -1521,7 +1524,7 @@
       <c r="E49">
         <v>6660</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>355.1951951951952</v>
       </c>
     </row>
@@ -1541,7 +1544,7 @@
       <c r="E50">
         <v>5308</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="2">
         <v>749.24642049736246</v>
       </c>
     </row>
@@ -1561,7 +1564,7 @@
       <c r="E51">
         <v>5289</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2">
         <v>559.67101531480432</v>
       </c>
     </row>
@@ -1581,7 +1584,7 @@
       <c r="E52">
         <v>5455</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="2">
         <v>509.09257561869839</v>
       </c>
     </row>
@@ -1601,7 +1604,7 @@
       <c r="E53">
         <v>5802</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="2">
         <v>786.59083074801788</v>
       </c>
     </row>
@@ -1621,7 +1624,7 @@
       <c r="E54">
         <v>6473</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="2">
         <v>264.32875019310978</v>
       </c>
     </row>
@@ -1641,7 +1644,7 @@
       <c r="E55">
         <v>5780</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2">
         <v>871.86851211072667</v>
       </c>
     </row>
@@ -1661,7 +1664,7 @@
       <c r="E56">
         <v>6894</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="2">
         <v>370.71366405570058</v>
       </c>
     </row>
@@ -1681,7 +1684,7 @@
       <c r="E57">
         <v>5982</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2">
         <v>552.10631895687061</v>
       </c>
     </row>
@@ -1701,7 +1704,7 @@
       <c r="E58">
         <v>5623</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="2">
         <v>344.67366174639869</v>
       </c>
     </row>
@@ -1721,7 +1724,7 @@
       <c r="E59">
         <v>6041</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="2">
         <v>638.47045191193513</v>
       </c>
     </row>
@@ -1741,7 +1744,7 @@
       <c r="E60">
         <v>5365</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="2">
         <v>766.26281453867659</v>
       </c>
     </row>
@@ -1761,7 +1764,7 @@
       <c r="E61">
         <v>6678</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="2">
         <v>517.47529200359384</v>
       </c>
     </row>
@@ -1781,7 +1784,7 @@
       <c r="E62">
         <v>6849</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="2">
         <v>395.0211709738648</v>
       </c>
     </row>
@@ -1801,7 +1804,7 @@
       <c r="E63">
         <v>6993</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="2">
         <v>447.50464750464749</v>
       </c>
     </row>
@@ -1821,7 +1824,7 @@
       <c r="E64">
         <v>6982</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="2">
         <v>314.65196218848467</v>
       </c>
     </row>
@@ -1841,7 +1844,7 @@
       <c r="E65">
         <v>5978</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="2">
         <v>461.82669789227162</v>
       </c>
     </row>
@@ -1861,7 +1864,7 @@
       <c r="E66">
         <v>5757</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="2">
         <v>560.86503387180824</v>
       </c>
     </row>
@@ -1881,7 +1884,7 @@
       <c r="E67">
         <v>6164</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="2">
         <v>544.58144062297208</v>
       </c>
     </row>
@@ -1901,7 +1904,7 @@
       <c r="E68">
         <v>5286</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="2">
         <v>816.0991297767689</v>
       </c>
     </row>
@@ -1921,7 +1924,7 @@
       <c r="E69">
         <v>6479</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="2">
         <v>434.95909862633118</v>
       </c>
     </row>
@@ -1941,7 +1944,7 @@
       <c r="E70">
         <v>6873</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="2">
         <v>218.91459333624331</v>
       </c>
     </row>
@@ -1961,7 +1964,7 @@
       <c r="E71">
         <v>6339</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="2">
         <v>474.36504180470109</v>
       </c>
     </row>
@@ -1981,7 +1984,7 @@
       <c r="E72">
         <v>5670</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="2">
         <v>568.69488536155211</v>
       </c>
     </row>
@@ -2001,7 +2004,7 @@
       <c r="E73">
         <v>6326</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="2">
         <v>700.06323110970595</v>
       </c>
     </row>
@@ -2021,7 +2024,7 @@
       <c r="E74">
         <v>5948</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="2">
         <v>708.72562205783458</v>
       </c>
     </row>
@@ -2041,7 +2044,7 @@
       <c r="E75">
         <v>6697</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="2">
         <v>407.94385545766761</v>
       </c>
     </row>
@@ -2061,7 +2064,7 @@
       <c r="E76">
         <v>5611</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="2">
         <v>685.52842630547138</v>
       </c>
     </row>
@@ -2081,7 +2084,7 @@
       <c r="E77">
         <v>6858</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="2">
         <v>284.93729950422858</v>
       </c>
     </row>
@@ -2101,7 +2104,7 @@
       <c r="E78">
         <v>6239</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="2">
         <v>455.12101298284978</v>
       </c>
     </row>
@@ -2121,7 +2124,7 @@
       <c r="E79">
         <v>6190</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="2">
         <v>798.35218093699507</v>
       </c>
     </row>
@@ -2141,7 +2144,7 @@
       <c r="E80">
         <v>5862</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="2">
         <v>514.39781644489938</v>
       </c>
     </row>
@@ -2161,7 +2164,7 @@
       <c r="E81">
         <v>6612</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="2">
         <v>419.43436176648521</v>
       </c>
     </row>
@@ -2181,7 +2184,7 @@
       <c r="E82">
         <v>5427</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="2">
         <v>709.28689883913762</v>
       </c>
     </row>
@@ -2201,7 +2204,7 @@
       <c r="E83">
         <v>6683</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="2">
         <v>238.5605267095616</v>
       </c>
     </row>
@@ -2221,7 +2224,7 @@
       <c r="E84">
         <v>5848</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="2">
         <v>438.64569083447338</v>
       </c>
     </row>
@@ -2241,7 +2244,7 @@
       <c r="E85">
         <v>6914</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="2">
         <v>478.8978883424935</v>
       </c>
     </row>
@@ -2261,7 +2264,7 @@
       <c r="E86">
         <v>5877</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="2">
         <v>511.41738982474061</v>
       </c>
     </row>
@@ -2281,7 +2284,7 @@
       <c r="E87">
         <v>6725</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="2">
         <v>425.02602230483268</v>
       </c>
     </row>
@@ -2301,7 +2304,7 @@
       <c r="E88">
         <v>5603</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="2">
         <v>739.56808852400502</v>
       </c>
     </row>
@@ -2321,7 +2324,7 @@
       <c r="E89">
         <v>5823</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="2">
         <v>310.57873948136699</v>
       </c>
     </row>
@@ -2341,7 +2344,7 @@
       <c r="E90">
         <v>5797</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="2">
         <v>443.8847679834397</v>
       </c>
     </row>
@@ -2361,7 +2364,7 @@
       <c r="E91">
         <v>5799</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="2">
         <v>323.03845490601827</v>
       </c>
     </row>
@@ -2381,7 +2384,7 @@
       <c r="E92">
         <v>6307</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="2">
         <v>428.79340415411451</v>
       </c>
     </row>
@@ -2401,7 +2404,7 @@
       <c r="E93">
         <v>5142</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="2">
         <v>532.16647218980938</v>
       </c>
     </row>
@@ -2421,7 +2424,7 @@
       <c r="E94">
         <v>6061</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="2">
         <v>497.52516086454381</v>
       </c>
     </row>
@@ -2441,7 +2444,7 @@
       <c r="E95">
         <v>5058</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="2">
         <v>525.74139976275205</v>
       </c>
     </row>
@@ -2461,7 +2464,7 @@
       <c r="E96">
         <v>5473</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="2">
         <v>658.41403252329621</v>
       </c>
     </row>
@@ -2481,7 +2484,7 @@
       <c r="E97">
         <v>6867</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="2">
         <v>632.60521333915824</v>
       </c>
     </row>
@@ -2501,7 +2504,7 @@
       <c r="E98">
         <v>5339</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="2">
         <v>530.66117250421428</v>
       </c>
     </row>
@@ -2521,7 +2524,7 @@
       <c r="E99">
         <v>5670</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="2">
         <v>408.09523809523807</v>
       </c>
     </row>
@@ -2541,7 +2544,7 @@
       <c r="E100">
         <v>6115</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="2">
         <v>592.85363859362224</v>
       </c>
     </row>
@@ -2561,7 +2564,7 @@
       <c r="E101">
         <v>5388</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="2">
         <v>598.47809948032659</v>
       </c>
     </row>
@@ -2581,7 +2584,7 @@
       <c r="E102">
         <v>5921</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="2">
         <v>530.45093734166528</v>
       </c>
     </row>
@@ -2601,7 +2604,7 @@
       <c r="E103">
         <v>5944</v>
       </c>
-      <c r="F103">
+      <c r="F103" s="2">
         <v>736.33916554508744</v>
       </c>
     </row>
@@ -2621,7 +2624,7 @@
       <c r="E104">
         <v>6273</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="2">
         <v>318.22094691535148</v>
       </c>
     </row>
@@ -2641,7 +2644,7 @@
       <c r="E105">
         <v>5127</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="2">
         <v>459.25492490735331</v>
       </c>
     </row>
@@ -2661,7 +2664,7 @@
       <c r="E106">
         <v>6339</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="2">
         <v>551.85360466950624</v>
       </c>
     </row>
@@ -2681,7 +2684,7 @@
       <c r="E107">
         <v>5186</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="2">
         <v>743.25106054762819</v>
       </c>
     </row>
@@ -2701,7 +2704,7 @@
       <c r="E108">
         <v>6144</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="2">
         <v>401.57877604166669</v>
       </c>
     </row>
@@ -2721,7 +2724,7 @@
       <c r="E109">
         <v>6534</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="2">
         <v>387.48086929905111</v>
       </c>
     </row>
@@ -2741,7 +2744,7 @@
       <c r="E110">
         <v>5400</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="2">
         <v>763.5</v>
       </c>
     </row>
@@ -2761,7 +2764,7 @@
       <c r="E111">
         <v>5500</v>
       </c>
-      <c r="F111">
+      <c r="F111" s="2">
         <v>632.38181818181818</v>
       </c>
     </row>
@@ -2781,7 +2784,7 @@
       <c r="E112">
         <v>6812</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="2">
         <v>420.91896652965357</v>
       </c>
     </row>
@@ -2801,7 +2804,7 @@
       <c r="E113">
         <v>5675</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="2">
         <v>590.23788546255503</v>
       </c>
     </row>
@@ -2821,7 +2824,7 @@
       <c r="E114">
         <v>5752</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="2">
         <v>671.62726008344919</v>
       </c>
     </row>
@@ -2841,7 +2844,7 @@
       <c r="E115">
         <v>5126</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="2">
         <v>683.57393679282086</v>
       </c>
     </row>
@@ -2861,7 +2864,7 @@
       <c r="E116">
         <v>5291</v>
       </c>
-      <c r="F116">
+      <c r="F116" s="2">
         <v>441.27764127764129</v>
       </c>
     </row>
@@ -2881,7 +2884,7 @@
       <c r="E117">
         <v>6347</v>
       </c>
-      <c r="F117">
+      <c r="F117" s="2">
         <v>669.65495509689617</v>
       </c>
     </row>
@@ -2901,7 +2904,7 @@
       <c r="E118">
         <v>6660</v>
       </c>
-      <c r="F118">
+      <c r="F118" s="2">
         <v>405.31531531531527</v>
       </c>
     </row>
@@ -2921,7 +2924,7 @@
       <c r="E119">
         <v>5812</v>
       </c>
-      <c r="F119">
+      <c r="F119" s="2">
         <v>403.1658637302134</v>
       </c>
     </row>
@@ -2941,7 +2944,7 @@
       <c r="E120">
         <v>6847</v>
       </c>
-      <c r="F120">
+      <c r="F120" s="2">
         <v>418.5044545056229</v>
       </c>
     </row>
@@ -2961,7 +2964,7 @@
       <c r="E121">
         <v>5985</v>
       </c>
-      <c r="F121">
+      <c r="F121" s="2">
         <v>790.17543859649118</v>
       </c>
     </row>
@@ -2981,7 +2984,7 @@
       <c r="E122">
         <v>5250</v>
       </c>
-      <c r="F122">
+      <c r="F122" s="2">
         <v>475.52380952380952</v>
       </c>
     </row>
@@ -3001,7 +3004,7 @@
       <c r="E123">
         <v>5540</v>
       </c>
-      <c r="F123">
+      <c r="F123" s="2">
         <v>627.23826714801453</v>
       </c>
     </row>
@@ -3021,7 +3024,7 @@
       <c r="E124">
         <v>5315</v>
       </c>
-      <c r="F124">
+      <c r="F124" s="2">
         <v>534.80714957666976</v>
       </c>
     </row>
@@ -3041,7 +3044,7 @@
       <c r="E125">
         <v>6633</v>
       </c>
-      <c r="F125">
+      <c r="F125" s="2">
         <v>479.6321423187095</v>
       </c>
     </row>
@@ -3061,7 +3064,7 @@
       <c r="E126">
         <v>6943</v>
       </c>
-      <c r="F126">
+      <c r="F126" s="2">
         <v>556.08526573527297</v>
       </c>
     </row>
@@ -3081,7 +3084,7 @@
       <c r="E127">
         <v>5921</v>
       </c>
-      <c r="F127">
+      <c r="F127" s="2">
         <v>355.58182739402127</v>
       </c>
     </row>
@@ -3101,7 +3104,7 @@
       <c r="E128">
         <v>5855</v>
       </c>
-      <c r="F128">
+      <c r="F128" s="2">
         <v>475.28608027327073</v>
       </c>
     </row>
@@ -3121,7 +3124,7 @@
       <c r="E129">
         <v>6480</v>
       </c>
-      <c r="F129">
+      <c r="F129" s="2">
         <v>344.5679012345679</v>
       </c>
     </row>
@@ -3141,7 +3144,7 @@
       <c r="E130">
         <v>5846</v>
       </c>
-      <c r="F130">
+      <c r="F130" s="2">
         <v>731.30345535408821</v>
       </c>
     </row>
@@ -3161,7 +3164,7 @@
       <c r="E131">
         <v>6425</v>
       </c>
-      <c r="F131">
+      <c r="F131" s="2">
         <v>413.97665369649809</v>
       </c>
     </row>
@@ -3181,7 +3184,7 @@
       <c r="E132">
         <v>6038</v>
       </c>
-      <c r="F132">
+      <c r="F132" s="2">
         <v>381.18582312023852</v>
       </c>
     </row>
@@ -3201,7 +3204,7 @@
       <c r="E133">
         <v>6520</v>
       </c>
-      <c r="F133">
+      <c r="F133" s="2">
         <v>627.28527607361957</v>
       </c>
     </row>
@@ -3221,7 +3224,7 @@
       <c r="E134">
         <v>6827</v>
       </c>
-      <c r="F134">
+      <c r="F134" s="2">
         <v>284.57594844001761</v>
       </c>
     </row>
@@ -3241,7 +3244,7 @@
       <c r="E135">
         <v>5307</v>
       </c>
-      <c r="F135">
+      <c r="F135" s="2">
         <v>536.53664970793295</v>
       </c>
     </row>
@@ -3261,7 +3264,7 @@
       <c r="E136">
         <v>5809</v>
       </c>
-      <c r="F136">
+      <c r="F136" s="2">
         <v>556.94611809261494</v>
       </c>
     </row>
@@ -3281,7 +3284,7 @@
       <c r="E137">
         <v>5444</v>
       </c>
-      <c r="F137">
+      <c r="F137" s="2">
         <v>934.2027920646583</v>
       </c>
     </row>
@@ -3301,7 +3304,7 @@
       <c r="E138">
         <v>5238</v>
       </c>
-      <c r="F138">
+      <c r="F138" s="2">
         <v>844.94081710576552</v>
       </c>
     </row>
@@ -3321,7 +3324,7 @@
       <c r="E139">
         <v>6728</v>
       </c>
-      <c r="F139">
+      <c r="F139" s="2">
         <v>234.3638525564804</v>
       </c>
     </row>
@@ -3341,7 +3344,7 @@
       <c r="E140">
         <v>6497</v>
       </c>
-      <c r="F140">
+      <c r="F140" s="2">
         <v>540.5879636755426</v>
       </c>
     </row>
@@ -3361,7 +3364,7 @@
       <c r="E141">
         <v>5202</v>
       </c>
-      <c r="F141">
+      <c r="F141" s="2">
         <v>723.64475201845448</v>
       </c>
     </row>
@@ -3381,7 +3384,7 @@
       <c r="E142">
         <v>6414</v>
       </c>
-      <c r="F142">
+      <c r="F142" s="2">
         <v>361.86467103211731</v>
       </c>
     </row>
@@ -3401,7 +3404,7 @@
       <c r="E143">
         <v>5632</v>
       </c>
-      <c r="F143">
+      <c r="F143" s="2">
         <v>462.97940340909088</v>
       </c>
     </row>
@@ -3421,7 +3424,7 @@
       <c r="E144">
         <v>6280</v>
       </c>
-      <c r="F144">
+      <c r="F144" s="2">
         <v>726.01910828025473</v>
       </c>
     </row>
@@ -3441,7 +3444,7 @@
       <c r="E145">
         <v>5488</v>
       </c>
-      <c r="F145">
+      <c r="F145" s="2">
         <v>377.0408163265306</v>
       </c>
     </row>
@@ -3461,7 +3464,7 @@
       <c r="E146">
         <v>6175</v>
       </c>
-      <c r="F146">
+      <c r="F146" s="2">
         <v>454.83400809716602</v>
       </c>
     </row>
@@ -3481,7 +3484,7 @@
       <c r="E147">
         <v>6886</v>
       </c>
-      <c r="F147">
+      <c r="F147" s="2">
         <v>435.46325878594251</v>
       </c>
     </row>
@@ -3501,7 +3504,7 @@
       <c r="E148">
         <v>6507</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="2">
         <v>634.9162440448747</v>
       </c>
     </row>
@@ -3521,7 +3524,7 @@
       <c r="E149">
         <v>5410</v>
       </c>
-      <c r="F149">
+      <c r="F149" s="2">
         <v>707.28280961182998</v>
       </c>
     </row>
@@ -3541,7 +3544,7 @@
       <c r="E150">
         <v>6512</v>
       </c>
-      <c r="F150">
+      <c r="F150" s="2">
         <v>723.37223587223582</v>
       </c>
     </row>
@@ -3561,7 +3564,7 @@
       <c r="E151">
         <v>5306</v>
       </c>
-      <c r="F151">
+      <c r="F151" s="2">
         <v>576.1779117979645</v>
       </c>
     </row>
@@ -3581,7 +3584,7 @@
       <c r="E152">
         <v>6451</v>
       </c>
-      <c r="F152">
+      <c r="F152" s="2">
         <v>538.8311889629515</v>
       </c>
     </row>
@@ -3601,7 +3604,7 @@
       <c r="E153">
         <v>5527</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="2">
         <v>769.22381038538083</v>
       </c>
     </row>
@@ -3621,7 +3624,7 @@
       <c r="E154">
         <v>6635</v>
       </c>
-      <c r="F154">
+      <c r="F154" s="2">
         <v>551.3489073097212</v>
       </c>
     </row>
@@ -3641,7 +3644,7 @@
       <c r="E155">
         <v>5471</v>
       </c>
-      <c r="F155">
+      <c r="F155" s="2">
         <v>531.310546518004</v>
       </c>
     </row>
@@ -3661,7 +3664,7 @@
       <c r="E156">
         <v>6386</v>
       </c>
-      <c r="F156">
+      <c r="F156" s="2">
         <v>719.08863138114634</v>
       </c>
     </row>
@@ -3681,7 +3684,7 @@
       <c r="E157">
         <v>6758</v>
       </c>
-      <c r="F157">
+      <c r="F157" s="2">
         <v>376.27996448653448</v>
       </c>
     </row>
@@ -3701,7 +3704,7 @@
       <c r="E158">
         <v>6535</v>
       </c>
-      <c r="F158">
+      <c r="F158" s="2">
         <v>389.76281560826322</v>
       </c>
     </row>
@@ -3721,7 +3724,7 @@
       <c r="E159">
         <v>6977</v>
       </c>
-      <c r="F159">
+      <c r="F159" s="2">
         <v>437.06464096316472</v>
       </c>
     </row>
@@ -3741,7 +3744,7 @@
       <c r="E160">
         <v>5946</v>
       </c>
-      <c r="F160">
+      <c r="F160" s="2">
         <v>566.2293979145644</v>
       </c>
     </row>
@@ -3761,7 +3764,7 @@
       <c r="E161">
         <v>5038</v>
       </c>
-      <c r="F161">
+      <c r="F161" s="2">
         <v>486.80031758634368</v>
       </c>
     </row>
@@ -3781,7 +3784,7 @@
       <c r="E162">
         <v>5149</v>
       </c>
-      <c r="F162">
+      <c r="F162" s="2">
         <v>774.84948533695865</v>
       </c>
     </row>
@@ -3801,7 +3804,7 @@
       <c r="E163">
         <v>6210</v>
       </c>
-      <c r="F163">
+      <c r="F163" s="2">
         <v>443.97745571658618</v>
       </c>
     </row>
@@ -3821,7 +3824,7 @@
       <c r="E164">
         <v>6874</v>
       </c>
-      <c r="F164">
+      <c r="F164" s="2">
         <v>290.06400931044521</v>
       </c>
     </row>
@@ -3841,7 +3844,7 @@
       <c r="E165">
         <v>5395</v>
       </c>
-      <c r="F165">
+      <c r="F165" s="2">
         <v>470.52826691380909</v>
       </c>
     </row>
@@ -3861,7 +3864,7 @@
       <c r="E166">
         <v>6530</v>
       </c>
-      <c r="F166">
+      <c r="F166" s="2">
         <v>604.18070444104137</v>
       </c>
     </row>
@@ -3881,7 +3884,7 @@
       <c r="E167">
         <v>6389</v>
       </c>
-      <c r="F167">
+      <c r="F167" s="2">
         <v>513.72671779621214</v>
       </c>
     </row>
@@ -3901,7 +3904,7 @@
       <c r="E168">
         <v>6253</v>
       </c>
-      <c r="F168">
+      <c r="F168" s="2">
         <v>654.78970094354713</v>
       </c>
     </row>
@@ -3921,7 +3924,7 @@
       <c r="E169">
         <v>6967</v>
       </c>
-      <c r="F169">
+      <c r="F169" s="2">
         <v>620.45356681498492</v>
       </c>
     </row>
@@ -3941,7 +3944,7 @@
       <c r="E170">
         <v>6484</v>
       </c>
-      <c r="F170">
+      <c r="F170" s="2">
         <v>409.05305367057372</v>
       </c>
     </row>
@@ -3961,7 +3964,7 @@
       <c r="E171">
         <v>5999</v>
       </c>
-      <c r="F171">
+      <c r="F171" s="2">
         <v>374.49574929154858</v>
       </c>
     </row>
@@ -3981,7 +3984,7 @@
       <c r="E172">
         <v>5415</v>
       </c>
-      <c r="F172">
+      <c r="F172" s="2">
         <v>600.42474607571557</v>
       </c>
     </row>
@@ -4001,7 +4004,7 @@
       <c r="E173">
         <v>5316</v>
       </c>
-      <c r="F173">
+      <c r="F173" s="2">
         <v>445.74868322046649</v>
       </c>
     </row>
@@ -4021,7 +4024,7 @@
       <c r="E174">
         <v>6875</v>
       </c>
-      <c r="F174">
+      <c r="F174" s="2">
         <v>400.77090909090907</v>
       </c>
     </row>
@@ -4041,7 +4044,7 @@
       <c r="E175">
         <v>5028</v>
       </c>
-      <c r="F175">
+      <c r="F175" s="2">
         <v>348.98568019093079</v>
       </c>
     </row>
@@ -4061,7 +4064,7 @@
       <c r="E176">
         <v>6007</v>
       </c>
-      <c r="F176">
+      <c r="F176" s="2">
         <v>522.20742467121693</v>
       </c>
     </row>
@@ -4081,7 +4084,7 @@
       <c r="E177">
         <v>5979</v>
       </c>
-      <c r="F177">
+      <c r="F177" s="2">
         <v>758.9730724201371</v>
       </c>
     </row>
@@ -4101,7 +4104,7 @@
       <c r="E178">
         <v>6353</v>
       </c>
-      <c r="F178">
+      <c r="F178" s="2">
         <v>758.53927278451124</v>
       </c>
     </row>
@@ -4121,7 +4124,7 @@
       <c r="E179">
         <v>5301</v>
       </c>
-      <c r="F179">
+      <c r="F179" s="2">
         <v>429.1265798905867</v>
       </c>
     </row>
@@ -4141,7 +4144,7 @@
       <c r="E180">
         <v>5166</v>
       </c>
-      <c r="F180">
+      <c r="F180" s="2">
         <v>854.80061943476574</v>
       </c>
     </row>
@@ -4161,7 +4164,7 @@
       <c r="E181">
         <v>6897</v>
       </c>
-      <c r="F181">
+      <c r="F181" s="2">
         <v>337.23357981731192</v>
       </c>
     </row>
@@ -4181,7 +4184,7 @@
       <c r="E182">
         <v>6266</v>
       </c>
-      <c r="F182">
+      <c r="F182" s="2">
         <v>460.72454516437921</v>
       </c>
     </row>
@@ -4201,7 +4204,7 @@
       <c r="E183">
         <v>6890</v>
       </c>
-      <c r="F183">
+      <c r="F183" s="2">
         <v>538.95500725689408</v>
       </c>
     </row>
@@ -4221,7 +4224,7 @@
       <c r="E184">
         <v>6622</v>
       </c>
-      <c r="F184">
+      <c r="F184" s="2">
         <v>348.9429175475687</v>
       </c>
     </row>
@@ -4241,7 +4244,7 @@
       <c r="E185">
         <v>5938</v>
       </c>
-      <c r="F185">
+      <c r="F185" s="2">
         <v>406.50050522061298</v>
       </c>
     </row>
@@ -4261,7 +4264,7 @@
       <c r="E186">
         <v>6701</v>
       </c>
-      <c r="F186">
+      <c r="F186" s="2">
         <v>599.56722877182506</v>
       </c>
     </row>
@@ -4281,7 +4284,7 @@
       <c r="E187">
         <v>5880</v>
       </c>
-      <c r="F187">
+      <c r="F187" s="2">
         <v>448.19727891156458</v>
       </c>
     </row>
@@ -4301,7 +4304,7 @@
       <c r="E188">
         <v>5206</v>
       </c>
-      <c r="F188">
+      <c r="F188" s="2">
         <v>888.68613138686123</v>
       </c>
     </row>
@@ -4321,7 +4324,7 @@
       <c r="E189">
         <v>6365</v>
       </c>
-      <c r="F189">
+      <c r="F189" s="2">
         <v>419.76433621366851</v>
       </c>
     </row>
@@ -4341,7 +4344,7 @@
       <c r="E190">
         <v>6234</v>
       </c>
-      <c r="F190">
+      <c r="F190" s="2">
         <v>383.14084055181257</v>
       </c>
     </row>
@@ -4361,7 +4364,7 @@
       <c r="E191">
         <v>6546</v>
       </c>
-      <c r="F191">
+      <c r="F191" s="2">
         <v>601.11518484570729</v>
       </c>
     </row>
@@ -4381,7 +4384,7 @@
       <c r="E192">
         <v>6681</v>
       </c>
-      <c r="F192">
+      <c r="F192" s="2">
         <v>421.35907798233802</v>
       </c>
     </row>
@@ -4401,7 +4404,7 @@
       <c r="E193">
         <v>6204</v>
       </c>
-      <c r="F193">
+      <c r="F193" s="2">
         <v>530.43197936814965</v>
       </c>
     </row>
@@ -4421,7 +4424,7 @@
       <c r="E194">
         <v>6759</v>
       </c>
-      <c r="F194">
+      <c r="F194" s="2">
         <v>433.48128421364112</v>
       </c>
     </row>
@@ -4441,7 +4444,7 @@
       <c r="E195">
         <v>6575</v>
       </c>
-      <c r="F195">
+      <c r="F195" s="2">
         <v>603.74144486692012</v>
       </c>
     </row>
@@ -4461,7 +4464,7 @@
       <c r="E196">
         <v>6023</v>
       </c>
-      <c r="F196">
+      <c r="F196" s="2">
         <v>399.50190934750123</v>
       </c>
     </row>
@@ -4481,7 +4484,7 @@
       <c r="E197">
         <v>6342</v>
       </c>
-      <c r="F197">
+      <c r="F197" s="2">
         <v>458.89309366130561</v>
       </c>
     </row>
@@ -4501,7 +4504,7 @@
       <c r="E198">
         <v>5617</v>
       </c>
-      <c r="F198">
+      <c r="F198" s="2">
         <v>615.61331671710877</v>
       </c>
     </row>
@@ -4521,7 +4524,7 @@
       <c r="E199">
         <v>5872</v>
       </c>
-      <c r="F199">
+      <c r="F199" s="2">
         <v>369.87397820163488</v>
       </c>
     </row>
@@ -4541,7 +4544,7 @@
       <c r="E200">
         <v>6926</v>
       </c>
-      <c r="F200">
+      <c r="F200" s="2">
         <v>600.21657522379439</v>
       </c>
     </row>
@@ -4561,7 +4564,7 @@
       <c r="E201">
         <v>5333</v>
       </c>
-      <c r="F201">
+      <c r="F201" s="2">
         <v>528.14550909431841</v>
       </c>
     </row>
@@ -4581,7 +4584,7 @@
       <c r="E202">
         <v>6851</v>
       </c>
-      <c r="F202">
+      <c r="F202" s="2">
         <v>470.29630710845129</v>
       </c>
     </row>
@@ -4601,7 +4604,7 @@
       <c r="E203">
         <v>6629</v>
       </c>
-      <c r="F203">
+      <c r="F203" s="2">
         <v>306.35088248604609</v>
       </c>
     </row>
@@ -4621,7 +4624,7 @@
       <c r="E204">
         <v>6313</v>
       </c>
-      <c r="F204">
+      <c r="F204" s="2">
         <v>765.68984634880405</v>
       </c>
     </row>
@@ -4641,7 +4644,7 @@
       <c r="E205">
         <v>6128</v>
       </c>
-      <c r="F205">
+      <c r="F205" s="2">
         <v>319.63120104438639</v>
       </c>
     </row>
@@ -4661,7 +4664,7 @@
       <c r="E206">
         <v>6262</v>
       </c>
-      <c r="F206">
+      <c r="F206" s="2">
         <v>644.04343660172469</v>
       </c>
     </row>
@@ -4681,7 +4684,7 @@
       <c r="E207">
         <v>6368</v>
       </c>
-      <c r="F207">
+      <c r="F207" s="2">
         <v>392.25816582914581</v>
       </c>
     </row>
@@ -4701,7 +4704,7 @@
       <c r="E208">
         <v>6259</v>
       </c>
-      <c r="F208">
+      <c r="F208" s="2">
         <v>558.30004793097942</v>
       </c>
     </row>
@@ -4721,7 +4724,7 @@
       <c r="E209">
         <v>5373</v>
       </c>
-      <c r="F209">
+      <c r="F209" s="2">
         <v>701.41447980643954</v>
       </c>
     </row>
@@ -4741,7 +4744,7 @@
       <c r="E210">
         <v>5458</v>
       </c>
-      <c r="F210">
+      <c r="F210" s="2">
         <v>798.35104433858555</v>
       </c>
     </row>
@@ -4761,7 +4764,7 @@
       <c r="E211">
         <v>6634</v>
       </c>
-      <c r="F211">
+      <c r="F211" s="2">
         <v>575.68586071751588</v>
       </c>
     </row>
@@ -4781,7 +4784,7 @@
       <c r="E212">
         <v>6308</v>
       </c>
-      <c r="F212">
+      <c r="F212" s="2">
         <v>569.61001902346231</v>
       </c>
     </row>
@@ -4801,7 +4804,7 @@
       <c r="E213">
         <v>6997</v>
       </c>
-      <c r="F213">
+      <c r="F213" s="2">
         <v>535.60097184507651</v>
       </c>
     </row>
@@ -4821,7 +4824,7 @@
       <c r="E214">
         <v>5393</v>
       </c>
-      <c r="F214">
+      <c r="F214" s="2">
         <v>819.87761913591692</v>
       </c>
     </row>
@@ -4841,7 +4844,7 @@
       <c r="E215">
         <v>5410</v>
       </c>
-      <c r="F215">
+      <c r="F215" s="2">
         <v>879.85212569316081</v>
       </c>
     </row>
@@ -4861,7 +4864,7 @@
       <c r="E216">
         <v>5165</v>
       </c>
-      <c r="F216">
+      <c r="F216" s="2">
         <v>748.15101645692164</v>
       </c>
     </row>
@@ -4881,7 +4884,7 @@
       <c r="E217">
         <v>6084</v>
       </c>
-      <c r="F217">
+      <c r="F217" s="2">
         <v>411.78500986193302</v>
       </c>
     </row>
@@ -4901,7 +4904,7 @@
       <c r="E218">
         <v>6019</v>
       </c>
-      <c r="F218">
+      <c r="F218" s="2">
         <v>458.71407210500081</v>
       </c>
     </row>
@@ -4921,7 +4924,7 @@
       <c r="E219">
         <v>5965</v>
       </c>
-      <c r="F219">
+      <c r="F219" s="2">
         <v>455.27242246437561</v>
       </c>
     </row>
@@ -4941,7 +4944,7 @@
       <c r="E220">
         <v>6578</v>
       </c>
-      <c r="F220">
+      <c r="F220" s="2">
         <v>537.48859835816359</v>
       </c>
     </row>
@@ -4961,7 +4964,7 @@
       <c r="E221">
         <v>5582</v>
       </c>
-      <c r="F221">
+      <c r="F221" s="2">
         <v>614.83339304908634</v>
       </c>
     </row>
@@ -4981,7 +4984,7 @@
       <c r="E222">
         <v>5328</v>
       </c>
-      <c r="F222">
+      <c r="F222" s="2">
         <v>499.62462462462457</v>
       </c>
     </row>
@@ -5001,7 +5004,7 @@
       <c r="E223">
         <v>5248</v>
       </c>
-      <c r="F223">
+      <c r="F223" s="2">
         <v>818.3498475609756</v>
       </c>
     </row>
@@ -5021,7 +5024,7 @@
       <c r="E224">
         <v>5947</v>
       </c>
-      <c r="F224">
+      <c r="F224" s="2">
         <v>741.65125273247008</v>
       </c>
     </row>
@@ -5041,7 +5044,7 @@
       <c r="E225">
         <v>5250</v>
       </c>
-      <c r="F225">
+      <c r="F225" s="2">
         <v>860.20952380952383</v>
       </c>
     </row>
@@ -5061,7 +5064,7 @@
       <c r="E226">
         <v>5473</v>
       </c>
-      <c r="F226">
+      <c r="F226" s="2">
         <v>418.63694500274067</v>
       </c>
     </row>
@@ -5081,7 +5084,7 @@
       <c r="E227">
         <v>6965</v>
       </c>
-      <c r="F227">
+      <c r="F227" s="2">
         <v>317.94687724335972</v>
       </c>
     </row>
@@ -5101,7 +5104,7 @@
       <c r="E228">
         <v>5912</v>
       </c>
-      <c r="F228">
+      <c r="F228" s="2">
         <v>383.94790257104188</v>
       </c>
     </row>
@@ -5121,7 +5124,7 @@
       <c r="E229">
         <v>5105</v>
       </c>
-      <c r="F229">
+      <c r="F229" s="2">
         <v>662.82076395690501</v>
       </c>
     </row>
@@ -5141,7 +5144,7 @@
       <c r="E230">
         <v>5733</v>
       </c>
-      <c r="F230">
+      <c r="F230" s="2">
         <v>739.21158206872497</v>
       </c>
     </row>
@@ -5161,7 +5164,7 @@
       <c r="E231">
         <v>6751</v>
       </c>
-      <c r="F231">
+      <c r="F231" s="2">
         <v>701.36276107243373</v>
       </c>
     </row>
@@ -5181,7 +5184,7 @@
       <c r="E232">
         <v>6961</v>
       </c>
-      <c r="F232">
+      <c r="F232" s="2">
         <v>479.85921562993832</v>
       </c>
     </row>
@@ -5201,7 +5204,7 @@
       <c r="E233">
         <v>6279</v>
       </c>
-      <c r="F233">
+      <c r="F233" s="2">
         <v>566.79407548972767</v>
       </c>
     </row>
@@ -5221,7 +5224,7 @@
       <c r="E234">
         <v>6497</v>
       </c>
-      <c r="F234">
+      <c r="F234" s="2">
         <v>430.87578882561178</v>
       </c>
     </row>
@@ -5241,7 +5244,7 @@
       <c r="E235">
         <v>6695</v>
       </c>
-      <c r="F235">
+      <c r="F235" s="2">
         <v>449.52949962658698</v>
       </c>
     </row>
@@ -5261,7 +5264,7 @@
       <c r="E236">
         <v>5921</v>
       </c>
-      <c r="F236">
+      <c r="F236" s="2">
         <v>334.4874176659348</v>
       </c>
     </row>
@@ -5281,7 +5284,7 @@
       <c r="E237">
         <v>5219</v>
       </c>
-      <c r="F237">
+      <c r="F237" s="2">
         <v>368.63383789998079</v>
       </c>
     </row>
@@ -5301,7 +5304,7 @@
       <c r="E238">
         <v>6942</v>
       </c>
-      <c r="F238">
+      <c r="F238" s="2">
         <v>521.07461826562951</v>
       </c>
     </row>
@@ -5321,7 +5324,7 @@
       <c r="E239">
         <v>6712</v>
       </c>
-      <c r="F239">
+      <c r="F239" s="2">
         <v>473.56972586412388</v>
       </c>
     </row>
@@ -5341,7 +5344,7 @@
       <c r="E240">
         <v>5793</v>
       </c>
-      <c r="F240">
+      <c r="F240" s="2">
         <v>289.60814776454339</v>
       </c>
     </row>
@@ -5361,7 +5364,7 @@
       <c r="E241">
         <v>5840</v>
       </c>
-      <c r="F241">
+      <c r="F241" s="2">
         <v>483.59589041095887</v>
       </c>
     </row>
@@ -5381,7 +5384,7 @@
       <c r="E242">
         <v>5133</v>
       </c>
-      <c r="F242">
+      <c r="F242" s="2">
         <v>580.96629651276055</v>
       </c>
     </row>
@@ -5401,7 +5404,7 @@
       <c r="E243">
         <v>5321</v>
       </c>
-      <c r="F243">
+      <c r="F243" s="2">
         <v>864.55553467393338</v>
       </c>
     </row>
@@ -5421,7 +5424,7 @@
       <c r="E244">
         <v>6683</v>
       </c>
-      <c r="F244">
+      <c r="F244" s="2">
         <v>300.38904683525362</v>
       </c>
     </row>
@@ -5441,7 +5444,7 @@
       <c r="E245">
         <v>6140</v>
       </c>
-      <c r="F245">
+      <c r="F245" s="2">
         <v>735.43973941368085</v>
       </c>
     </row>
@@ -5461,7 +5464,7 @@
       <c r="E246">
         <v>5098</v>
       </c>
-      <c r="F246">
+      <c r="F246" s="2">
         <v>897.13613181639857</v>
       </c>
     </row>
@@ -5481,7 +5484,7 @@
       <c r="E247">
         <v>5798</v>
       </c>
-      <c r="F247">
+      <c r="F247" s="2">
         <v>816.88513280441532</v>
       </c>
     </row>
@@ -5501,7 +5504,7 @@
       <c r="E248">
         <v>6818</v>
       </c>
-      <c r="F248">
+      <c r="F248" s="2">
         <v>509.15224405984162</v>
       </c>
     </row>
@@ -5521,7 +5524,7 @@
       <c r="E249">
         <v>6742</v>
       </c>
-      <c r="F249">
+      <c r="F249" s="2">
         <v>525.64520913675472</v>
       </c>
     </row>
@@ -5541,7 +5544,7 @@
       <c r="E250">
         <v>5152</v>
       </c>
-      <c r="F250">
+      <c r="F250" s="2">
         <v>577.71739130434787</v>
       </c>
     </row>
@@ -5561,7 +5564,7 @@
       <c r="E251">
         <v>6890</v>
       </c>
-      <c r="F251">
+      <c r="F251" s="2">
         <v>281.611030478955</v>
       </c>
     </row>
@@ -5581,7 +5584,7 @@
       <c r="E252">
         <v>5270</v>
       </c>
-      <c r="F252">
+      <c r="F252" s="2">
         <v>539.46869070208732</v>
       </c>
     </row>
@@ -5601,7 +5604,7 @@
       <c r="E253">
         <v>5028</v>
       </c>
-      <c r="F253">
+      <c r="F253" s="2">
         <v>562.70883054892602</v>
       </c>
     </row>
@@ -5621,7 +5624,7 @@
       <c r="E254">
         <v>6694</v>
       </c>
-      <c r="F254">
+      <c r="F254" s="2">
         <v>273.48371676127869</v>
       </c>
     </row>
@@ -5641,7 +5644,7 @@
       <c r="E255">
         <v>6033</v>
       </c>
-      <c r="F255">
+      <c r="F255" s="2">
         <v>405.42018896071602</v>
       </c>
     </row>
@@ -5661,7 +5664,7 @@
       <c r="E256">
         <v>5978</v>
       </c>
-      <c r="F256">
+      <c r="F256" s="2">
         <v>591.50217464034802</v>
       </c>
     </row>
@@ -5681,7 +5684,7 @@
       <c r="E257">
         <v>5641</v>
       </c>
-      <c r="F257">
+      <c r="F257" s="2">
         <v>773.74578975358986</v>
       </c>
     </row>
@@ -5701,7 +5704,7 @@
       <c r="E258">
         <v>6015</v>
       </c>
-      <c r="F258">
+      <c r="F258" s="2">
         <v>678.35411471321686</v>
       </c>
     </row>
@@ -5721,7 +5724,7 @@
       <c r="E259">
         <v>5534</v>
       </c>
-      <c r="F259">
+      <c r="F259" s="2">
         <v>378.83989880737261</v>
       </c>
     </row>
@@ -5741,7 +5744,7 @@
       <c r="E260">
         <v>5823</v>
       </c>
-      <c r="F260">
+      <c r="F260" s="2">
         <v>515.35291087068526</v>
       </c>
     </row>
@@ -5761,7 +5764,7 @@
       <c r="E261">
         <v>6020</v>
       </c>
-      <c r="F261">
+      <c r="F261" s="2">
         <v>629.03654485049833</v>
       </c>
     </row>
@@ -5781,7 +5784,7 @@
       <c r="E262">
         <v>5878</v>
       </c>
-      <c r="F262">
+      <c r="F262" s="2">
         <v>310.82000680503569</v>
       </c>
     </row>
@@ -5801,7 +5804,7 @@
       <c r="E263">
         <v>6014</v>
       </c>
-      <c r="F263">
+      <c r="F263" s="2">
         <v>583.95410708347185</v>
       </c>
     </row>
@@ -5821,7 +5824,7 @@
       <c r="E264">
         <v>6172</v>
       </c>
-      <c r="F264">
+      <c r="F264" s="2">
         <v>535.82307193778354</v>
       </c>
     </row>
@@ -5841,7 +5844,7 @@
       <c r="E265">
         <v>5203</v>
       </c>
-      <c r="F265">
+      <c r="F265" s="2">
         <v>591.58177974245621</v>
       </c>
     </row>
@@ -5861,7 +5864,7 @@
       <c r="E266">
         <v>6048</v>
       </c>
-      <c r="F266">
+      <c r="F266" s="2">
         <v>425.74404761904759</v>
       </c>
     </row>
@@ -5881,7 +5884,7 @@
       <c r="E267">
         <v>5863</v>
       </c>
-      <c r="F267">
+      <c r="F267" s="2">
         <v>488.60651543578371</v>
       </c>
     </row>
@@ -5901,7 +5904,7 @@
       <c r="E268">
         <v>5506</v>
       </c>
-      <c r="F268">
+      <c r="F268" s="2">
         <v>575.97166727206684</v>
       </c>
     </row>
@@ -5921,7 +5924,7 @@
       <c r="E269">
         <v>5355</v>
       </c>
-      <c r="F269">
+      <c r="F269" s="2">
         <v>469.80392156862752</v>
       </c>
     </row>
@@ -5941,7 +5944,7 @@
       <c r="E270">
         <v>6446</v>
       </c>
-      <c r="F270">
+      <c r="F270" s="2">
         <v>781.24418243872174</v>
       </c>
     </row>
@@ -5961,7 +5964,7 @@
       <c r="E271">
         <v>6354</v>
       </c>
-      <c r="F271">
+      <c r="F271" s="2">
         <v>425.77903682719551</v>
       </c>
     </row>
@@ -5981,7 +5984,7 @@
       <c r="E272">
         <v>5555</v>
       </c>
-      <c r="F272">
+      <c r="F272" s="2">
         <v>689.73897389738977</v>
       </c>
     </row>
@@ -6001,7 +6004,7 @@
       <c r="E273">
         <v>5121</v>
       </c>
-      <c r="F273">
+      <c r="F273" s="2">
         <v>771.91954696348364</v>
       </c>
     </row>
@@ -6021,7 +6024,7 @@
       <c r="E274">
         <v>5788</v>
       </c>
-      <c r="F274">
+      <c r="F274" s="2">
         <v>736.92121630960617</v>
       </c>
     </row>
@@ -6041,7 +6044,7 @@
       <c r="E275">
         <v>6564</v>
       </c>
-      <c r="F275">
+      <c r="F275" s="2">
         <v>315.53930530164541</v>
       </c>
     </row>
@@ -6061,7 +6064,7 @@
       <c r="E276">
         <v>5996</v>
       </c>
-      <c r="F276">
+      <c r="F276" s="2">
         <v>329.63642428285527</v>
       </c>
     </row>
@@ -6081,7 +6084,7 @@
       <c r="E277">
         <v>6323</v>
       </c>
-      <c r="F277">
+      <c r="F277" s="2">
         <v>320.74964415625487</v>
       </c>
     </row>
@@ -6101,7 +6104,7 @@
       <c r="E278">
         <v>6220</v>
       </c>
-      <c r="F278">
+      <c r="F278" s="2">
         <v>636.14147909967846</v>
       </c>
     </row>
@@ -6121,7 +6124,7 @@
       <c r="E279">
         <v>6274</v>
       </c>
-      <c r="F279">
+      <c r="F279" s="2">
         <v>476.61778769525017</v>
       </c>
     </row>
@@ -6141,7 +6144,7 @@
       <c r="E280">
         <v>6931</v>
       </c>
-      <c r="F280">
+      <c r="F280" s="2">
         <v>682.94618381185978</v>
       </c>
     </row>
@@ -6161,7 +6164,7 @@
       <c r="E281">
         <v>5770</v>
       </c>
-      <c r="F281">
+      <c r="F281" s="2">
         <v>708.02426343154241</v>
       </c>
     </row>
@@ -6181,7 +6184,7 @@
       <c r="E282">
         <v>6229</v>
       </c>
-      <c r="F282">
+      <c r="F282" s="2">
         <v>385.4711831754696</v>
       </c>
     </row>
@@ -6201,7 +6204,7 @@
       <c r="E283">
         <v>5769</v>
       </c>
-      <c r="F283">
+      <c r="F283" s="2">
         <v>630.03986826139715</v>
       </c>
     </row>
@@ -6221,7 +6224,7 @@
       <c r="E284">
         <v>6450</v>
       </c>
-      <c r="F284">
+      <c r="F284" s="2">
         <v>356.38759689922477</v>
       </c>
     </row>
@@ -6241,7 +6244,7 @@
       <c r="E285">
         <v>6526</v>
       </c>
-      <c r="F285">
+      <c r="F285" s="2">
         <v>355.83818571866379</v>
       </c>
     </row>
@@ -6261,7 +6264,7 @@
       <c r="E286">
         <v>5625</v>
       </c>
-      <c r="F286">
+      <c r="F286" s="2">
         <v>719.87555555555559</v>
       </c>
     </row>
@@ -6281,7 +6284,7 @@
       <c r="E287">
         <v>6953</v>
       </c>
-      <c r="F287">
+      <c r="F287" s="2">
         <v>467.46728031065732</v>
       </c>
     </row>
@@ -6301,7 +6304,7 @@
       <c r="E288">
         <v>6210</v>
       </c>
-      <c r="F288">
+      <c r="F288" s="2">
         <v>707.42351046698877</v>
       </c>
     </row>
@@ -6321,7 +6324,7 @@
       <c r="E289">
         <v>6885</v>
       </c>
-      <c r="F289">
+      <c r="F289" s="2">
         <v>343.29702251270879</v>
       </c>
     </row>

</xml_diff>